<commit_message>
Feat: Parking lot & telegram
</commit_message>
<xml_diff>
--- a/src/twitter-like/capacity.xlsx
+++ b/src/twitter-like/capacity.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\u-Boulanger\home\utkusarioglu\dev\workshops\system-design-workshop\src\twitter-like\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C438E5-C953-45CA-A039-FD3D1121E4AD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7105C903-6D78-4EA2-B993-A76F7B448C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20370" windowHeight="10125" activeTab="4" xr2:uid="{556F4A94-5C9C-4358-BA95-CA85D8105C43}"/>
-    <workbookView visibility="hidden" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" activeTab="1" xr2:uid="{CB29EB16-430D-49A7-ACD6-E296A78C93BA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{556F4A94-5C9C-4358-BA95-CA85D8105C43}"/>
+    <workbookView visibility="hidden" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CB29EB16-430D-49A7-ACD6-E296A78C93BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Specifications" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,19 @@
     <sheet name="Daily Storage" sheetId="11" r:id="rId4"/>
     <sheet name="Outstanding Storage" sheetId="10" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2005,7 +2014,7 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -2456,7 +2465,7 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -2808,6 +2817,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>